<commit_message>
La till testfall för ekvivalensklasserna. Fixed indentation in Command
</commit_message>
<xml_diff>
--- a/Testning/Ekvivalensklasser.xlsx
+++ b/Testning/Ekvivalensklasser.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Ekvivalensklasser" sheetId="1" r:id="rId1"/>
+    <sheet name="Testfall" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="149">
   <si>
     <t>ID</t>
   </si>
@@ -41,9 +41,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>validFIleName</t>
-  </si>
-  <si>
     <t>innehåller &lt;</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>innehåller \</t>
   </si>
   <si>
-    <t>257 tecken</t>
-  </si>
-  <si>
     <t>slutar på .txt</t>
   </si>
   <si>
@@ -83,12 +77,6 @@
     <t>innehåller mellanslag</t>
   </si>
   <si>
-    <t>1-255 korrekta tecken</t>
-  </si>
-  <si>
-    <t>256 korrekta tecken</t>
-  </si>
-  <si>
     <t>fil finns redan</t>
   </si>
   <si>
@@ -98,9 +86,6 @@
     <t>touchFile</t>
   </si>
   <si>
-    <t>validFSOName</t>
-  </si>
-  <si>
     <t>mapp finns</t>
   </si>
   <si>
@@ -119,9 +104,6 @@
     <t>Gränsvärde</t>
   </si>
   <si>
-    <t>0 tecken</t>
-  </si>
-  <si>
     <t>TF1</t>
   </si>
   <si>
@@ -134,62 +116,365 @@
     <t>TP2</t>
   </si>
   <si>
-    <t>VFN1</t>
-  </si>
-  <si>
-    <t>VFN2</t>
-  </si>
-  <si>
-    <t>VFN3</t>
-  </si>
-  <si>
-    <t>VFN4</t>
-  </si>
-  <si>
-    <t>VFN5</t>
-  </si>
-  <si>
-    <t>VFN6</t>
-  </si>
-  <si>
-    <t>VFN7</t>
-  </si>
-  <si>
-    <t>VFN8</t>
-  </si>
-  <si>
-    <t>VFN9</t>
-  </si>
-  <si>
-    <t>VFN10</t>
-  </si>
-  <si>
-    <t>VFN11</t>
-  </si>
-  <si>
-    <t>VFN12</t>
-  </si>
-  <si>
-    <t>VFN13</t>
-  </si>
-  <si>
-    <t>VFN14</t>
-  </si>
-  <si>
-    <t>VFN15</t>
-  </si>
-  <si>
-    <t>VFN16</t>
-  </si>
-  <si>
-    <t>VFSON</t>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Testar klass</t>
+  </si>
+  <si>
+    <t>TP3</t>
+  </si>
+  <si>
+    <t>ingen sökväg</t>
+  </si>
+  <si>
+    <t>fil.txt</t>
+  </si>
+  <si>
+    <t>fil skapas</t>
+  </si>
+  <si>
+    <t>1-254 korrekta tecken</t>
+  </si>
+  <si>
+    <t>255 korrekta tecken</t>
+  </si>
+  <si>
+    <t>&lt;5 tecken</t>
+  </si>
+  <si>
+    <t>256 tecken</t>
+  </si>
+  <si>
+    <t>6-254 korrekta tecken</t>
+  </si>
+  <si>
+    <t>5 korrekta tecken</t>
+  </si>
+  <si>
+    <t>validFile</t>
+  </si>
+  <si>
+    <t>VF11</t>
+  </si>
+  <si>
+    <t>VF12</t>
+  </si>
+  <si>
+    <t>VF15</t>
+  </si>
+  <si>
+    <t>VF1</t>
+  </si>
+  <si>
+    <t>VF10</t>
+  </si>
+  <si>
+    <t>VF13</t>
+  </si>
+  <si>
+    <t>VF14</t>
+  </si>
+  <si>
+    <t>VF16</t>
+  </si>
+  <si>
+    <t>VF2</t>
+  </si>
+  <si>
+    <t>VF3</t>
+  </si>
+  <si>
+    <t>VF4</t>
+  </si>
+  <si>
+    <t>VF5</t>
+  </si>
+  <si>
+    <t>VF6</t>
+  </si>
+  <si>
+    <t>VF7</t>
+  </si>
+  <si>
+    <t>VF8</t>
+  </si>
+  <si>
+    <t>VF9</t>
+  </si>
+  <si>
+    <t>VF17</t>
+  </si>
+  <si>
+    <t>TP3, TF2, VF11, VF15</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>[mapp 255 tecken] a.txt</t>
+  </si>
+  <si>
+    <t>Mapp finns</t>
+  </si>
+  <si>
+    <t>Fil finns</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4</t>
+  </si>
+  <si>
+    <t>T1, T2</t>
+  </si>
+  <si>
+    <t>TP2, VF18, TF2</t>
+  </si>
+  <si>
+    <t>fil skapas, mapp skapas</t>
+  </si>
+  <si>
+    <t>T2, T4</t>
+  </si>
+  <si>
+    <t>TP1, VF12</t>
+  </si>
+  <si>
+    <t>/mapp [filnamn 254 tecken (.txt)]</t>
+  </si>
+  <si>
+    <t>/mapp [filnamn 255 tecken (.txt)]</t>
+  </si>
+  <si>
+    <t>&lt;abc.txt</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>ogiltigt filnamn</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>a bc.txt</t>
+  </si>
+  <si>
+    <t>[256 tecken (.txt)</t>
+  </si>
+  <si>
+    <t>.txt</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>&gt;abc.txt</t>
+  </si>
+  <si>
+    <t>:abc.txt</t>
+  </si>
+  <si>
+    <t>"abc.txt</t>
+  </si>
+  <si>
+    <t>/abc.txt</t>
+  </si>
+  <si>
+    <t>|abc.txt</t>
+  </si>
+  <si>
+    <t>?abc.txt</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>T23</t>
+  </si>
+  <si>
+    <t>T24</t>
+  </si>
+  <si>
+    <t>T25</t>
+  </si>
+  <si>
+    <t>T26</t>
+  </si>
+  <si>
+    <t>T27</t>
+  </si>
+  <si>
+    <t>T28</t>
+  </si>
+  <si>
+    <t>T29</t>
+  </si>
+  <si>
+    <t>*abc.txt</t>
+  </si>
+  <si>
+    <t>\abc.txt</t>
+  </si>
+  <si>
+    <t>ma\\pp fil.txt</t>
+  </si>
+  <si>
+    <t>validPath</t>
+  </si>
+  <si>
+    <t>VP1</t>
+  </si>
+  <si>
+    <t>VP2</t>
+  </si>
+  <si>
+    <t>VP10</t>
+  </si>
+  <si>
+    <t>VP11</t>
+  </si>
+  <si>
+    <t>VP12</t>
+  </si>
+  <si>
+    <t>VP3</t>
+  </si>
+  <si>
+    <t>VP4</t>
+  </si>
+  <si>
+    <t>VP5</t>
+  </si>
+  <si>
+    <t>VP6</t>
+  </si>
+  <si>
+    <t>VP7</t>
+  </si>
+  <si>
+    <t>VP8</t>
+  </si>
+  <si>
+    <t>VP9</t>
+  </si>
+  <si>
+    <t>TP1, VF11, VF15, VP1, TF2</t>
+  </si>
+  <si>
+    <t>innehåller \\</t>
+  </si>
+  <si>
+    <t>ogiltigt path</t>
+  </si>
+  <si>
+    <t>ma pp fil.txt</t>
+  </si>
+  <si>
+    <t>[256 tecken] fil.txt</t>
+  </si>
+  <si>
+    <t>ma&lt;pp fil.txt</t>
+  </si>
+  <si>
+    <t>ma&gt;pp fil.txt</t>
+  </si>
+  <si>
+    <t>ma:pp fil.txt</t>
+  </si>
+  <si>
+    <t>ma"pp fil.txt</t>
+  </si>
+  <si>
+    <t>ma|pp fil.txt</t>
+  </si>
+  <si>
+    <t>ma?pp fil.txt</t>
+  </si>
+  <si>
+    <t>ma*pp fil.txt</t>
+  </si>
+  <si>
+    <t>absolut sökväg</t>
+  </si>
+  <si>
+    <t>/mapp/mapp2 fil.txt</t>
+  </si>
+  <si>
+    <t>skapar fil</t>
+  </si>
+  <si>
+    <t>TP1, VF11, TF2, VF15, VP12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +537,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -267,7 +560,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -313,6 +606,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -325,11 +629,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -361,10 +666,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F34" totalsRowShown="0">
-  <autoFilter ref="A2:F34"/>
-  <sortState ref="A3:E33">
-    <sortCondition ref="B2:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F37" totalsRowShown="0">
+  <autoFilter ref="A2:F37"/>
+  <sortState ref="A3:F38">
+    <sortCondition ref="D2:D38"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="ID"/>
@@ -375,6 +680,22 @@
     <tableColumn id="7" name="Kommentar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:G31" totalsRowShown="0">
+  <autoFilter ref="A2:G31"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="7" name="Mapp finns"/>
+    <tableColumn id="6" name="Fil finns"/>
+    <tableColumn id="2" name="Input"/>
+    <tableColumn id="3" name="Output"/>
+    <tableColumn id="4" name="Testar klass"/>
+    <tableColumn id="5" name="Kommentar"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -691,27 +1012,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.375" customWidth="1"/>
-    <col min="3" max="3" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.375" customWidth="1"/>
+    <col min="5" max="5" width="18.375" customWidth="1"/>
     <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -736,395 +1055,545 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>145</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
-        <v>15</v>
+      <c r="E15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>31</v>
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="F19" t="s">
-        <v>31</v>
+      <c r="E19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>134</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>41</v>
+      </c>
+      <c r="E30" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1141,13 +1610,548 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="28.875" customWidth="1"/>
+    <col min="8" max="8" width="51.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Information om hur touch funkar i dagsläget och hur det skall funka utifrån de nya testfallen
</commit_message>
<xml_diff>
--- a/Testning/Ekvivalensklasser.xlsx
+++ b/Testning/Ekvivalensklasser.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ekvivalensklasser" sheetId="1" r:id="rId1"/>
     <sheet name="Testfall" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Info" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -245,12 +245,6 @@
     <t>T7</t>
   </si>
   <si>
-    <t>T1, T2, T3, T4</t>
-  </si>
-  <si>
-    <t>T1, T2</t>
-  </si>
-  <si>
     <t>TP2, VF18, TF2</t>
   </si>
   <si>
@@ -311,9 +305,6 @@
     <t>a bc.txt</t>
   </si>
   <si>
-    <t>[256 tecken (.txt)</t>
-  </si>
-  <si>
     <t>.txt</t>
   </si>
   <si>
@@ -468,13 +459,84 @@
   </si>
   <si>
     <t>TP1, VF11, TF2, VF15, VP12</t>
+  </si>
+  <si>
+    <t>TP4</t>
+  </si>
+  <si>
+    <t>mappar finns ej, skapas</t>
+  </si>
+  <si>
+    <t>skapar båda mapparna, skapar filen</t>
+  </si>
+  <si>
+    <t>[256 tecken (.txt)]</t>
+  </si>
+  <si>
+    <t>T30</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4, T30</t>
+  </si>
+  <si>
+    <t>T1, T2, T30</t>
+  </si>
+  <si>
+    <t>T2, T30</t>
+  </si>
+  <si>
+    <t>T29, T30</t>
+  </si>
+  <si>
+    <t>TF2, TP4, VF15, VF11, VP1, VP12</t>
+  </si>
+  <si>
+    <t>Touch funkar i dagsläget (2016-10-24)</t>
+  </si>
+  <si>
+    <t>Touch ska funka:</t>
+  </si>
+  <si>
+    <t>Skapa fil i mappen man är i, förutsatt att filnamnet är korrekt angett (validFileName)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Man kan antingen ange bara filnamn, och då skapar den filen i mappen man står i, 
+eller så anger man en mapp/sökväg innan filnamnet. Filen skapas då i den mappen. 
+Finns inte mappen/mapparna skapas den/de
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Exempel: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Mapparna finns ej, absolut sökväg: "/mapp/mapp2 fil.txt" - varken mapparna eller filen finns, så allt skapas
+Mapp finns ej: "mapp fil.txt" - mappen skapas i nuvarande mapp och filen skapas i den nya mappen
+Nuvarande mapp: "fil.txt" - filen skapas i nuvarande mapp</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,8 +607,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,6 +626,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,12 +705,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -666,8 +757,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F37" totalsRowShown="0">
-  <autoFilter ref="A2:F37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F38" totalsRowShown="0">
+  <autoFilter ref="A2:F38"/>
   <sortState ref="A3:F38">
     <sortCondition ref="D2:D38"/>
   </sortState>
@@ -684,8 +775,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:G31" totalsRowShown="0">
-  <autoFilter ref="A2:G31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:G32" totalsRowShown="0">
+  <autoFilter ref="A2:G32"/>
   <tableColumns count="7">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="7" name="Mapp finns"/>
@@ -1012,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1029,14 +1120,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1072,7 +1163,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1089,7 +1180,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1128,93 +1219,90 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
         <v>26</v>
@@ -1222,19 +1310,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="F12" t="s">
         <v>26</v>
@@ -1242,358 +1330,378 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>69</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>142</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
         <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
         <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
         <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
         <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" t="s">
         <v>13</v>
       </c>
-      <c r="E37" t="s">
-        <v>115</v>
+      <c r="E38" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1610,13 +1718,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1630,7 +1738,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1682,13 +1790,13 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1699,10 +1807,10 @@
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1713,13 +1821,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1747,10 +1855,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
         <v>82</v>
-      </c>
-      <c r="E8" t="s">
-        <v>84</v>
       </c>
       <c r="F8" t="s">
         <v>48</v>
@@ -1764,10 +1872,10 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F9" t="s">
         <v>49</v>
@@ -1775,16 +1883,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
         <v>50</v>
@@ -1792,16 +1900,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
@@ -1809,16 +1917,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F12" t="s">
         <v>52</v>
@@ -1826,16 +1934,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s">
         <v>53</v>
@@ -1843,16 +1951,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
         <v>54</v>
@@ -1860,16 +1968,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
         <v>55</v>
@@ -1877,16 +1985,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F16" t="s">
         <v>56</v>
@@ -1894,16 +2002,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F17" t="s">
         <v>57</v>
@@ -1911,16 +2019,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
         <v>58</v>
@@ -1928,16 +2036,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F19" t="s">
         <v>59</v>
@@ -1945,16 +2053,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s">
         <v>60</v>
@@ -1962,189 +2070,203 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F28" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" t="s">
+        <v>143</v>
+      </c>
+      <c r="E32" t="s">
         <v>148</v>
+      </c>
+      <c r="F32" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2157,12 +2279,83 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:H5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tests for Touch from equivalenceclasses
</commit_message>
<xml_diff>
--- a/Testning/Ekvivalensklasser.xlsx
+++ b/Testning/Ekvivalensklasser.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ekvivalensklasser" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -263,9 +263,6 @@
     <t>/mapp [filnamn 255 tecken (.txt)]</t>
   </si>
   <si>
-    <t>&lt;abc.txt</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -302,33 +299,9 @@
     <t>T17</t>
   </si>
   <si>
-    <t>a bc.txt</t>
-  </si>
-  <si>
     <t>.txt</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>&gt;abc.txt</t>
-  </si>
-  <si>
-    <t>:abc.txt</t>
-  </si>
-  <si>
-    <t>"abc.txt</t>
-  </si>
-  <si>
-    <t>/abc.txt</t>
-  </si>
-  <si>
-    <t>|abc.txt</t>
-  </si>
-  <si>
-    <t>?abc.txt</t>
-  </si>
-  <si>
     <t>T18</t>
   </si>
   <si>
@@ -365,12 +338,6 @@
     <t>T29</t>
   </si>
   <si>
-    <t>*abc.txt</t>
-  </si>
-  <si>
-    <t>\abc.txt</t>
-  </si>
-  <si>
     <t>ma\\pp fil.txt</t>
   </si>
   <si>
@@ -455,9 +422,6 @@
     <t>/mapp/mapp2 fil.txt</t>
   </si>
   <si>
-    <t>skapar fil</t>
-  </si>
-  <si>
     <t>TP1, VF11, TF2, VF15, VP12</t>
   </si>
   <si>
@@ -465,9 +429,6 @@
   </si>
   <si>
     <t>mappar finns ej, skapas</t>
-  </si>
-  <si>
-    <t>skapar båda mapparna, skapar filen</t>
   </si>
   <si>
     <t>[256 tecken (.txt)]</t>
@@ -530,6 +491,117 @@
 Mapp finns ej: "mapp fil.txt" - mappen skapas i nuvarande mapp och filen skapas i den nya mappen
 Nuvarande mapp: "fil.txt" - filen skapas i nuvarande mapp</t>
     </r>
+  </si>
+  <si>
+    <t>Testnamn</t>
+  </si>
+  <si>
+    <t>&lt;fil.txt</t>
+  </si>
+  <si>
+    <t>f il.txt</t>
+  </si>
+  <si>
+    <t>fil</t>
+  </si>
+  <si>
+    <t>&gt;fil.txt</t>
+  </si>
+  <si>
+    <t>:fil.txt</t>
+  </si>
+  <si>
+    <t>"fil.txt</t>
+  </si>
+  <si>
+    <t>/fil.txt</t>
+  </si>
+  <si>
+    <t>|fil.txt</t>
+  </si>
+  <si>
+    <t>?fil.txt</t>
+  </si>
+  <si>
+    <t>*fil.txt</t>
+  </si>
+  <si>
+    <t>\fil.txt</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_fileAlreadyExists()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharSmaller()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharSpace()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_toLong()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_toShort()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_wrongFileType()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharBigger()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharColon()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharQuote()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharSlash()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doCommand_fileName_invalidCharBar() </t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharQuestion()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharAsterisk()</t>
+  </si>
+  <si>
+    <t>doCommand_fileName_invalidCharBackslash()</t>
+  </si>
+  <si>
+    <t>doCommand_path_toLong()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharSmaller()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharSpace()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharBigger()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharColon()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharQuote()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharBar()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharQuestion()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharAsterisk()</t>
+  </si>
+  <si>
+    <t>doCommand_path_invalidCharBackslash()</t>
+  </si>
+  <si>
+    <t>Båda mapparna och fil skapas</t>
   </si>
 </sst>
 </file>
@@ -708,13 +780,16 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -722,9 +797,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -775,15 +847,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:G32" totalsRowShown="0">
-  <autoFilter ref="A2:G32"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H32" totalsRowShown="0">
+  <autoFilter ref="A2:H32"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="7" name="Mapp finns"/>
     <tableColumn id="6" name="Fil finns"/>
     <tableColumn id="2" name="Input"/>
     <tableColumn id="3" name="Output"/>
     <tableColumn id="4" name="Testar klass"/>
+    <tableColumn id="8" name="Testnamn"/>
     <tableColumn id="5" name="Kommentar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1120,14 +1193,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1163,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1219,19 +1292,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1248,7 +1321,7 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1285,7 +1358,7 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1310,10 +1383,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -1322,7 +1395,7 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="F12" t="s">
         <v>26</v>
@@ -1330,10 +1403,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
@@ -1350,19 +1423,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1418,7 +1491,7 @@
         <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
         <v>26</v>
@@ -1435,7 +1508,7 @@
         <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1449,7 +1522,7 @@
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1463,7 +1536,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1477,7 +1550,7 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1491,7 +1564,7 @@
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1505,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1519,7 +1592,7 @@
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1533,7 +1606,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1547,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1561,147 +1634,147 @@
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
         <v>120</v>
       </c>
-      <c r="B29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C29" t="s">
-        <v>131</v>
-      </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1718,13 +1791,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1732,17 +1805,18 @@
     <col min="1" max="1" width="4.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.875" customWidth="1"/>
-    <col min="8" max="8" width="51.875" customWidth="1"/>
+    <col min="7" max="7" width="40.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1762,10 +1836,13 @@
         <v>33</v>
       </c>
       <c r="G2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1782,7 +1859,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1796,10 +1873,10 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1813,7 +1890,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -1830,7 +1907,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1846,8 +1923,11 @@
       <c r="F7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1855,16 +1935,19 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -1872,407 +1955,474 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F20" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>103</v>
       </c>
-      <c r="C21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" t="s">
+        <v>118</v>
+      </c>
+      <c r="G30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
         <v>132</v>
       </c>
-      <c r="F21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" t="s">
         <v>133</v>
       </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" t="s">
         <v>132</v>
       </c>
-      <c r="F22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" t="s">
-        <v>134</v>
-      </c>
-      <c r="E23" t="s">
-        <v>132</v>
-      </c>
-      <c r="F23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" t="s">
-        <v>136</v>
-      </c>
-      <c r="E25" t="s">
-        <v>132</v>
-      </c>
-      <c r="F25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" t="s">
-        <v>137</v>
-      </c>
-      <c r="E26" t="s">
-        <v>132</v>
-      </c>
-      <c r="F26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" t="s">
-        <v>132</v>
-      </c>
-      <c r="F27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" t="s">
-        <v>139</v>
-      </c>
-      <c r="E28" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" t="s">
-        <v>140</v>
-      </c>
-      <c r="E29" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" t="s">
-        <v>141</v>
-      </c>
-      <c r="E30" t="s">
-        <v>132</v>
-      </c>
-      <c r="F30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>143</v>
-      </c>
-      <c r="E31" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>150</v>
-      </c>
-      <c r="D32" t="s">
-        <v>143</v>
-      </c>
       <c r="E32" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="F32" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2281,72 +2431,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9" style="4"/>
+    <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="A1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="A2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="A4" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="A5" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Fyllde på slutrapporten med verktyg, påbörjad skiss över design, alltom ekvivalensklasser förutom testfall.Gjorde tabell över testfall och påbörjade klassdiagram. Tillsammans med övriga.
</commit_message>
<xml_diff>
--- a/Testning/Ekvivalensklasser.xlsx
+++ b/Testning/Ekvivalensklasser.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ekvivalensklasser" sheetId="1" r:id="rId1"/>
     <sheet name="Testfall" sheetId="2" r:id="rId2"/>
-    <sheet name="Info" sheetId="3" r:id="rId3"/>
+    <sheet name="Testmatris" sheetId="4" r:id="rId3"/>
+    <sheet name="Info" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -245,18 +247,12 @@
     <t>T7</t>
   </si>
   <si>
-    <t>TP2, VF18, TF2</t>
-  </si>
-  <si>
     <t>fil skapas, mapp skapas</t>
   </si>
   <si>
     <t>T2, T4</t>
   </si>
   <si>
-    <t>TP1, VF12</t>
-  </si>
-  <si>
     <t>/mapp [filnamn 254 tecken (.txt)]</t>
   </si>
   <si>
@@ -378,9 +374,6 @@
   </si>
   <si>
     <t>VP9</t>
-  </si>
-  <si>
-    <t>TP1, VF11, VF15, VP1, TF2</t>
   </si>
   <si>
     <t>innehåller \\</t>
@@ -603,12 +596,36 @@
   <si>
     <t>Båda mapparna och fil skapas</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>VP13</t>
+  </si>
+  <si>
+    <t>TP1, VF11, VF15, VP1, TF2, TP3</t>
+  </si>
+  <si>
+    <t>TP2, VF18, TF2, TP3</t>
+  </si>
+  <si>
+    <t>TP1, VF12, TP3</t>
+  </si>
+  <si>
+    <t>TF1, TP3</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4, T5</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,8 +704,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -707,8 +739,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -765,6 +803,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -777,7 +824,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -798,6 +845,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -810,7 +862,25 @@
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="7" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -832,7 +902,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F38" totalsRowShown="0">
   <autoFilter ref="A2:F38"/>
   <sortState ref="A3:F38">
-    <sortCondition ref="D2:D38"/>
+    <sortCondition ref="A2:A38"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="ID"/>
@@ -860,6 +930,45 @@
     <tableColumn id="5" name="Kommentar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:AE37" totalsRowShown="0">
+  <tableColumns count="31">
+    <tableColumn id="1" name=" " dataDxfId="0"/>
+    <tableColumn id="2" name="T1"/>
+    <tableColumn id="3" name="T2"/>
+    <tableColumn id="4" name="T3"/>
+    <tableColumn id="5" name="T4"/>
+    <tableColumn id="6" name="T5"/>
+    <tableColumn id="7" name="T6"/>
+    <tableColumn id="8" name="T7"/>
+    <tableColumn id="9" name="T8"/>
+    <tableColumn id="10" name="T9"/>
+    <tableColumn id="11" name="T10"/>
+    <tableColumn id="12" name="T11"/>
+    <tableColumn id="13" name="T12"/>
+    <tableColumn id="14" name="T13"/>
+    <tableColumn id="15" name="T14"/>
+    <tableColumn id="16" name="T15"/>
+    <tableColumn id="17" name="T16"/>
+    <tableColumn id="18" name="T17"/>
+    <tableColumn id="19" name="T18"/>
+    <tableColumn id="20" name="T19"/>
+    <tableColumn id="21" name="T20"/>
+    <tableColumn id="22" name="T21"/>
+    <tableColumn id="23" name="T22"/>
+    <tableColumn id="24" name="T23"/>
+    <tableColumn id="25" name="T24"/>
+    <tableColumn id="26" name="T25"/>
+    <tableColumn id="27" name="T26"/>
+    <tableColumn id="28" name="T27"/>
+    <tableColumn id="29" name="T28"/>
+    <tableColumn id="30" name="T29"/>
+    <tableColumn id="31" name="T30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1178,8 +1287,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1224,178 +1336,163 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
         <v>26</v>
@@ -1403,19 +1500,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
@@ -1423,215 +1517,224 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
         <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
         <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>90</v>
+        <v>137</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>93</v>
@@ -1642,139 +1745,148 @@
         <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>120</v>
+        <v>128</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>182</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>96</v>
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1793,12 +1905,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1836,7 +1949,7 @@
         <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -1867,13 +1980,13 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1884,10 +1997,10 @@
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1898,13 +2011,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1921,10 +2034,10 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>186</v>
       </c>
       <c r="G7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1935,16 +2048,16 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
         <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1955,467 +2068,467 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
         <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
         <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
         <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
         <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
         <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
         <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
         <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F18" t="s">
         <v>58</v>
       </c>
       <c r="G18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
         <v>59</v>
       </c>
       <c r="G19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
         <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F23" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="G23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G25" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G26" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G28" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G30" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E31" t="s">
         <v>37</v>
       </c>
       <c r="F31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E32" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F32" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2429,10 +2542,476 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.375" customWidth="1"/>
+    <col min="2" max="31" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T1" t="s">
+        <v>92</v>
+      </c>
+      <c r="U1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W1" t="s">
+        <v>95</v>
+      </c>
+      <c r="X1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="N19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="P21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="T26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="U27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="V29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="W31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="X32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2442,7 +3021,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2454,7 +3033,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2476,7 +3055,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2488,7 +3067,7 @@
     </row>
     <row r="5" spans="1:8" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>

</xml_diff>

<commit_message>
Uppdaterade rapporten med TDD för mig, Annika och Felix + fler test för touch utefter ekvivalensklasserna + sparade och la in det detaljerade klassdiagrammet som Felix tagit fram
</commit_message>
<xml_diff>
--- a/Testning/Ekvivalensklasser.xlsx
+++ b/Testning/Ekvivalensklasser.xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ekvivalensklasser" sheetId="1" r:id="rId1"/>
@@ -18,12 +17,12 @@
     <sheet name="Testmatris" sheetId="4" r:id="rId3"/>
     <sheet name="Info" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="190">
   <si>
     <t>ID</t>
   </si>
@@ -619,6 +618,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>doCommand_createFile_currentDir()</t>
   </si>
 </sst>
 </file>
@@ -833,6 +835,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -845,11 +852,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -918,7 +920,11 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H32" totalsRowShown="0">
-  <autoFilter ref="A2:H32"/>
+  <autoFilter ref="A2:H32">
+    <filterColumn colId="6">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="7" name="Mapp finns"/>
@@ -1287,11 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1305,14 +1308,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1905,13 +1908,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1971,6 +1973,9 @@
       <c r="F3" t="s">
         <v>62</v>
       </c>
+      <c r="G3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2020,7 +2025,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2040,7 +2045,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -2060,7 +2065,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -2080,7 +2085,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -2100,7 +2105,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -2120,7 +2125,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -2140,7 +2145,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -2160,7 +2165,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -2180,7 +2185,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -2200,7 +2205,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -2220,7 +2225,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -2240,7 +2245,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -2260,7 +2265,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -2280,7 +2285,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2300,7 +2305,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -2320,7 +2325,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2340,7 +2345,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -2360,7 +2365,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -2380,7 +2385,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -2400,7 +2405,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -2420,7 +2425,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -2440,7 +2445,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -2460,7 +2465,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -2480,7 +2485,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -2547,12 +2552,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2656,7 +2655,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F2" t="s">
@@ -2664,7 +2663,7 @@
       </c>
     </row>
     <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B3" t="s">
@@ -2684,7 +2683,7 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
@@ -2695,7 +2694,7 @@
       </c>
     </row>
     <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D5" t="s">
@@ -2703,7 +2702,7 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B6" t="s">
@@ -2723,7 +2722,7 @@
       </c>
     </row>
     <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>131</v>
       </c>
       <c r="AE7" t="s">
@@ -2731,7 +2730,7 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
       <c r="G8" t="s">
@@ -2739,7 +2738,7 @@
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>49</v>
       </c>
       <c r="H9" t="s">
@@ -2747,7 +2746,7 @@
       </c>
     </row>
     <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B10" t="s">
@@ -2761,7 +2760,7 @@
       </c>
     </row>
     <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E11" t="s">
@@ -2769,7 +2768,7 @@
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
       <c r="I12" t="s">
@@ -2777,7 +2776,7 @@
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
       <c r="J13" t="s">
@@ -2785,7 +2784,7 @@
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B14" t="s">
@@ -2805,7 +2804,7 @@
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="5" t="s">
         <v>52</v>
       </c>
       <c r="K15" t="s">
@@ -2813,7 +2812,7 @@
       </c>
     </row>
     <row r="16" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="8" t="s">
         <v>61</v>
       </c>
       <c r="D16" t="s">
@@ -2821,7 +2820,7 @@
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="5" t="s">
         <v>53</v>
       </c>
       <c r="L17" t="s">
@@ -2829,7 +2828,7 @@
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="4" t="s">
         <v>54</v>
       </c>
       <c r="M18" t="s">
@@ -2837,7 +2836,7 @@
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="5" t="s">
         <v>55</v>
       </c>
       <c r="N19" t="s">
@@ -2845,7 +2844,7 @@
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
       <c r="O20" t="s">
@@ -2853,7 +2852,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="5" t="s">
         <v>57</v>
       </c>
       <c r="P21" t="s">
@@ -2861,7 +2860,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
       <c r="Q22" t="s">
@@ -2869,7 +2868,7 @@
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="5" t="s">
         <v>59</v>
       </c>
       <c r="R23" t="s">
@@ -2877,7 +2876,7 @@
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="4" t="s">
         <v>60</v>
       </c>
       <c r="S24" t="s">
@@ -2885,7 +2884,7 @@
       </c>
     </row>
     <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C25" t="s">
@@ -2896,7 +2895,7 @@
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="4" t="s">
         <v>107</v>
       </c>
       <c r="T26" t="s">
@@ -2904,7 +2903,7 @@
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="5" t="s">
         <v>108</v>
       </c>
       <c r="U27" t="s">
@@ -2912,7 +2911,7 @@
       </c>
     </row>
     <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="8" t="s">
         <v>109</v>
       </c>
       <c r="AD28" t="s">
@@ -2923,7 +2922,7 @@
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="5" t="s">
         <v>182</v>
       </c>
       <c r="V29" t="s">
@@ -2931,7 +2930,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D30" t="s">
@@ -2939,7 +2938,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="5" t="s">
         <v>110</v>
       </c>
       <c r="W31" t="s">
@@ -2947,7 +2946,7 @@
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="4" t="s">
         <v>111</v>
       </c>
       <c r="X32" t="s">
@@ -2955,7 +2954,7 @@
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="5" t="s">
         <v>112</v>
       </c>
       <c r="Y33" t="s">
@@ -2963,7 +2962,7 @@
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="4" t="s">
         <v>113</v>
       </c>
       <c r="Z34" t="s">
@@ -2971,7 +2970,7 @@
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="5" t="s">
         <v>114</v>
       </c>
       <c r="AA35" t="s">
@@ -2979,7 +2978,7 @@
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="4" t="s">
         <v>115</v>
       </c>
       <c r="AB36" t="s">
@@ -2987,7 +2986,7 @@
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="6" t="s">
         <v>116</v>
       </c>
       <c r="AC37" t="s">
@@ -3010,9 +3009,6 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:H1"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3020,28 +3016,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -3054,28 +3050,28 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Skrev de sista testerna för touch utifrån ekvivalensklasserna + uppdaterade ekvivalensklasserna (dokumentet) + variabel för maxlängd för FSO + uppdaterade testfallen för bestlutstabell (tillsammans med övriga) + fyllde på slutrapporten med TDD-utvärdering, Pontus TDD, info om ekvivalensklasser och beslutstabeller, granskning, byggskript (tilsammans med övriga)
</commit_message>
<xml_diff>
--- a/Testning/Ekvivalensklasser.xlsx
+++ b/Testning/Ekvivalensklasser.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Ekvivalensklasser" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="195">
   <si>
     <t>ID</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Input</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>Testar klass</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>TP3, TF2, VF11, VF15</t>
   </si>
   <si>
-    <t>Precondition</t>
-  </si>
-  <si>
     <t>[mapp 255 tecken] a.txt</t>
   </si>
   <si>
@@ -250,12 +244,6 @@
   </si>
   <si>
     <t>T2, T4</t>
-  </si>
-  <si>
-    <t>/mapp [filnamn 254 tecken (.txt)]</t>
-  </si>
-  <si>
-    <t>/mapp [filnamn 255 tecken (.txt)]</t>
   </si>
   <si>
     <t>N/A</t>
@@ -614,20 +602,47 @@
     <t>TF1, TP3</t>
   </si>
   <si>
-    <t>T1, T2, T3, T4, T5</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>doCommand_createFile_currentDir()</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>doCommand_createFile_createDirs()</t>
+  </si>
+  <si>
+    <t>mapp [filnamn 255 tecken (.txt)]</t>
+  </si>
+  <si>
+    <t>doCommand_createFile_givenAbsolutePath()</t>
+  </si>
+  <si>
+    <t>doCommand_createFileMaxLength_givenPath()</t>
+  </si>
+  <si>
+    <t>T1, T5</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4, T29, T30</t>
+  </si>
+  <si>
+    <t>mapp fil.txt</t>
+  </si>
+  <si>
+    <t>doCommand_createFile_givenPath()</t>
+  </si>
+  <si>
+    <t>doCommand_createFile_createDirMaxLength()</t>
+  </si>
+  <si>
+    <t>Preconditions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,13 +723,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Arial"/>
@@ -826,7 +834,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -835,9 +843,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -852,6 +857,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -867,7 +874,7 @@
   <dxfs count="1">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -920,17 +927,12 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:H32" totalsRowShown="0">
-  <autoFilter ref="A2:H32">
-    <filterColumn colId="6">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="7" name="Mapp finns"/>
     <tableColumn id="6" name="Fil finns"/>
     <tableColumn id="2" name="Input"/>
-    <tableColumn id="3" name="Output"/>
+    <tableColumn id="3" name="Expected result"/>
     <tableColumn id="4" name="Testar klass"/>
     <tableColumn id="8" name="Testnamn"/>
     <tableColumn id="5" name="Kommentar"/>
@@ -1293,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1303,19 +1305,19 @@
     <col min="2" max="2" width="18.375" customWidth="1"/>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1348,7 +1350,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1365,7 +1367,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1382,7 +1384,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1399,103 +1401,103 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
         <v>26</v>
@@ -1503,16 +1505,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
@@ -1520,24 +1522,24 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -1546,38 +1548,38 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
@@ -1585,131 +1587,131 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F26" t="s">
         <v>26</v>
@@ -1717,78 +1719,78 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F31" t="s">
         <v>26</v>
@@ -1796,100 +1798,100 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1908,27 +1910,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.75" customWidth="1"/>
     <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.875" customWidth="1"/>
     <col min="7" max="7" width="40.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="51.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1936,22 +1940,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
       </c>
       <c r="E2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -1959,581 +1963,596 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>191</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>179</v>
+      </c>
+      <c r="G4" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>184</v>
+        <v>180</v>
+      </c>
+      <c r="G5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>186</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="G6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>145</v>
       </c>
-      <c r="E8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>146</v>
       </c>
-      <c r="E9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>90</v>
       </c>
-      <c r="E11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G23" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>155</v>
-      </c>
-      <c r="E20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E21" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>93</v>
       </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
         <v>119</v>
       </c>
-      <c r="E22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" t="s">
         <v>108</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" t="s">
-        <v>118</v>
-      </c>
-      <c r="F23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" t="s">
-        <v>110</v>
-      </c>
-      <c r="G24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>96</v>
       </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
         <v>122</v>
       </c>
-      <c r="E25" t="s">
-        <v>118</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" t="s">
         <v>111</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G29" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>97</v>
       </c>
-      <c r="C26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
         <v>123</v>
       </c>
-      <c r="E26" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E30" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" t="s">
         <v>112</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G30" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27" t="s">
-        <v>113</v>
-      </c>
-      <c r="G27" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" t="s">
-        <v>114</v>
-      </c>
-      <c r="G28" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G29" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" t="s">
-        <v>116</v>
-      </c>
-      <c r="G30" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="G31" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E32" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F32" t="s">
-        <v>139</v>
+        <v>135</v>
+      </c>
+      <c r="G32" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2549,445 +2568,439 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH21" sqref="AH21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.375" customWidth="1"/>
+    <col min="1" max="1" width="5.375" style="11" customWidth="1"/>
     <col min="2" max="31" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>181</v>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>177</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" t="s">
-        <v>73</v>
-      </c>
       <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>83</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>85</v>
       </c>
-      <c r="O1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>88</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>89</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" t="s">
         <v>91</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>92</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>93</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>94</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>95</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>96</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>97</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>98</v>
       </c>
-      <c r="AA1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="S24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="T26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="U27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="V29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="AE1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D6" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="K15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="P21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="R23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="S24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="W31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="T26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="X32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="U27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="Y33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="AD28" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="V29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="Z34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="W31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="AA35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="X32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="AB36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="AC37" t="s">
         <v>5</v>
@@ -3016,28 +3029,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="A1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="A2" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -3050,28 +3063,28 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="A4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
+      <c r="A5" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>